<commit_message>
Refactored code into utils
</commit_message>
<xml_diff>
--- a/output1.xlsx
+++ b/output1.xlsx
@@ -18,7 +18,7 @@
     <definedName name="posts1">backend!$A$305:$D$404</definedName>
     <definedName name="todos">backend!$A$103:$D$302</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" calcMode="auto" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -18045,7 +18045,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E100"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1:E10"/>
@@ -18271,9 +18271,7 @@
     </row>
     <row r="11">
       <c r="A11" s="3" t="n"/>
-      <c r="B11" s="3" t="n">
-        <v>10</v>
-      </c>
+      <c r="B11" s="3" t="n"/>
       <c r="C11" s="3">
         <f>SUM(C2:C10)</f>
         <v/>
@@ -18282,1163 +18280,6 @@
       <c r="E11" s="3">
         <f>sum(E1:E10)</f>
         <v/>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="n">
-        <v>11000</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>quam nostrum impedit mollitia quod et dolor</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>consequatur autem doloribus natus consectetur</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="B14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="n">
-        <v>13000</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>ab rerum non rerum consequatur ut ea unde</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="n">
-        <v>14000</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>ducimus molestias eos animi atque nihil</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>ut pariatur rerum ipsum natus repellendus praesentium</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="B17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C17" t="n">
-        <v>16000</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>voluptatem aut maxime inventore autem magnam atque repellat</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="n">
-        <v>17</v>
-      </c>
-      <c r="C18" t="n">
-        <v>17000</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>aut minima voluptatem ut velit</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="n">
-        <v>18</v>
-      </c>
-      <c r="C19" t="n">
-        <v>18000</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>nesciunt quia et doloremque</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="n">
-        <v>19</v>
-      </c>
-      <c r="C20" t="n">
-        <v>19000</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>velit pariatur quaerat similique libero omnis quia</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="n">
-        <v>20</v>
-      </c>
-      <c r="C21" t="n">
-        <v>20000</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>voluptas rerum iure ut enim</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="B22" t="n">
-        <v>21</v>
-      </c>
-      <c r="C22" t="n">
-        <v>21000</v>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>repudiandae voluptatem optio est consequatur rem in temporibus et</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="n">
-        <v>22</v>
-      </c>
-      <c r="C23" t="n">
-        <v>22000</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>et rem non provident vel ut</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="n">
-        <v>23</v>
-      </c>
-      <c r="C24" t="n">
-        <v>23000</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>incidunt quisquam hic adipisci sequi</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="n">
-        <v>24</v>
-      </c>
-      <c r="C25" t="n">
-        <v>24000</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>dolores ut et facere placeat</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="B26" t="n">
-        <v>25</v>
-      </c>
-      <c r="C26" t="n">
-        <v>25000</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>vero maxime id possimus sunt neque et consequatur</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="B27" t="n">
-        <v>26</v>
-      </c>
-      <c r="C27" t="n">
-        <v>26000</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>quibusdam saepe ipsa vel harum</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="n">
-        <v>27</v>
-      </c>
-      <c r="C28" t="n">
-        <v>27000</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>id non nostrum expedita</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" t="n">
-        <v>28</v>
-      </c>
-      <c r="C29" t="n">
-        <v>28000</v>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>omnis neque exercitationem sed dolor atque maxime aut cum</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="B30" t="n">
-        <v>29</v>
-      </c>
-      <c r="C30" t="n">
-        <v>29000</v>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>inventore ut quasi magnam itaque est fugit</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="B31" t="n">
-        <v>30</v>
-      </c>
-      <c r="C31" t="n">
-        <v>30000</v>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>tempora assumenda et similique odit distinctio error</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="n">
-        <v>31</v>
-      </c>
-      <c r="C32" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>adipisci laborum fuga laboriosam</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="n">
-        <v>32</v>
-      </c>
-      <c r="C33" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>reiciendis dolores a ut qui debitis non quo labore</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="n">
-        <v>33</v>
-      </c>
-      <c r="C34" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>iste eos nostrum</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="n">
-        <v>34</v>
-      </c>
-      <c r="C35" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>cumque voluptatibus rerum architecto blanditiis</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="n">
-        <v>35</v>
-      </c>
-      <c r="C36" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>et impedit nisi quae magni necessitatibus sed aut pariatur</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="n">
-        <v>36</v>
-      </c>
-      <c r="C37" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>nihil cupiditate voluptate neque</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" t="n">
-        <v>37</v>
-      </c>
-      <c r="C38" t="n">
-        <v>7000</v>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>est placeat dicta ut nisi rerum iste</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="n">
-        <v>38</v>
-      </c>
-      <c r="C39" t="n">
-        <v>8000</v>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>unde a sequi id</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="n">
-        <v>39</v>
-      </c>
-      <c r="C40" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>ratione porro illum labore eum aperiam sed</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" t="n">
-        <v>40</v>
-      </c>
-      <c r="C41" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>voluptas neque et sint aut quo odit</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="n">
-        <v>41</v>
-      </c>
-      <c r="C42" t="n">
-        <v>11000</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>ea voluptates maiores eos accusantium officiis tempore mollitia consequatur</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="n">
-        <v>42</v>
-      </c>
-      <c r="C43" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>tenetur explicabo ea</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="n">
-        <v>43</v>
-      </c>
-      <c r="C44" t="n">
-        <v>13000</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>aperiam doloremque nihil</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="n">
-        <v>44</v>
-      </c>
-      <c r="C45" t="n">
-        <v>14000</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>sapiente cum numquam officia consequatur vel natus quos suscipit</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="n">
-        <v>45</v>
-      </c>
-      <c r="C46" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>tenetur quos ea unde est enim corrupti qui</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="n">
-        <v>46</v>
-      </c>
-      <c r="C47" t="n">
-        <v>16000</v>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>molestiae voluptate non</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="n">
-        <v>47</v>
-      </c>
-      <c r="C48" t="n">
-        <v>17000</v>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>temporibus molestiae aut</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="n">
-        <v>48</v>
-      </c>
-      <c r="C49" t="n">
-        <v>18000</v>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>modi consequatur culpa aut quam soluta alias perspiciatis laudantium</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="n">
-        <v>49</v>
-      </c>
-      <c r="C50" t="n">
-        <v>19000</v>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>ut aut vero repudiandae voluptas ullam voluptas at consequatur</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="n">
-        <v>50</v>
-      </c>
-      <c r="C51" t="n">
-        <v>20000</v>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>sed qui sed quas sit ducimus dolor</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="n">
-        <v>51</v>
-      </c>
-      <c r="C52" t="n">
-        <v>21000</v>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>odit laboriosam sint quia cupiditate animi quis</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" t="n">
-        <v>52</v>
-      </c>
-      <c r="C53" t="n">
-        <v>22000</v>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>necessitatibus quas et sunt at voluptatem</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="n">
-        <v>53</v>
-      </c>
-      <c r="C54" t="n">
-        <v>23000</v>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>est vel sequi voluptatem nemo quam molestiae modi enim</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="n">
-        <v>54</v>
-      </c>
-      <c r="C55" t="n">
-        <v>24000</v>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>aut non illo amet perferendis</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="n">
-        <v>55</v>
-      </c>
-      <c r="C56" t="n">
-        <v>25000</v>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>qui culpa itaque omnis in nesciunt architecto error</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" t="n">
-        <v>56</v>
-      </c>
-      <c r="C57" t="n">
-        <v>26000</v>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>omnis qui maiores tempora officiis omnis rerum sed repellat</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" t="n">
-        <v>57</v>
-      </c>
-      <c r="C58" t="n">
-        <v>27000</v>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>libero excepturi voluptatem est architecto quae voluptatum officia tempora</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" t="n">
-        <v>58</v>
-      </c>
-      <c r="C59" t="n">
-        <v>28000</v>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>nulla illo consequatur aspernatur veritatis aut error delectus et</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" t="n">
-        <v>59</v>
-      </c>
-      <c r="C60" t="n">
-        <v>29000</v>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>eligendi similique provident nihil</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" t="n">
-        <v>60</v>
-      </c>
-      <c r="C61" t="n">
-        <v>30000</v>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>omnis mollitia sunt aliquid eum consequatur fugit minus laudantium</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" t="n">
-        <v>61</v>
-      </c>
-      <c r="C62" t="n">
-        <v>1000</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>delectus iusto et</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" t="n">
-        <v>62</v>
-      </c>
-      <c r="C63" t="n">
-        <v>2000</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>eos ea non recusandae iste ut quasi</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="n">
-        <v>63</v>
-      </c>
-      <c r="C64" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>velit est quam</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="n">
-        <v>64</v>
-      </c>
-      <c r="C65" t="n">
-        <v>4000</v>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>autem voluptatem amet iure quae</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="n">
-        <v>65</v>
-      </c>
-      <c r="C66" t="n">
-        <v>5000</v>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>voluptates delectus iure iste qui</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" t="n">
-        <v>66</v>
-      </c>
-      <c r="C67" t="n">
-        <v>6000</v>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>velit sed quia dolor dolores delectus</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" t="n">
-        <v>67</v>
-      </c>
-      <c r="C68" t="n">
-        <v>7000</v>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>ad voluptas nostrum et nihil</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" t="n">
-        <v>68</v>
-      </c>
-      <c r="C69" t="n">
-        <v>8000</v>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>qui quasi nihil aut voluptatum sit dolore minima</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="n">
-        <v>69</v>
-      </c>
-      <c r="C70" t="n">
-        <v>9000</v>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>qui aut est</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="B71" t="n">
-        <v>70</v>
-      </c>
-      <c r="C71" t="n">
-        <v>10000</v>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>et deleniti unde</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" t="n">
-        <v>71</v>
-      </c>
-      <c r="C72" t="n">
-        <v>11000</v>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>et vel corporis</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="n">
-        <v>72</v>
-      </c>
-      <c r="C73" t="n">
-        <v>12000</v>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>unde exercitationem ut</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" t="n">
-        <v>73</v>
-      </c>
-      <c r="C74" t="n">
-        <v>13000</v>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>quos omnis officia</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="n">
-        <v>74</v>
-      </c>
-      <c r="C75" t="n">
-        <v>14000</v>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>quia est eius vitae dolor</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="n">
-        <v>75</v>
-      </c>
-      <c r="C76" t="n">
-        <v>15000</v>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>aut quia expedita non</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="n">
-        <v>76</v>
-      </c>
-      <c r="C77" t="n">
-        <v>16000</v>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>dolorem magnam facere itaque ut reprehenderit tenetur corrupti</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="n">
-        <v>77</v>
-      </c>
-      <c r="C78" t="n">
-        <v>17000</v>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>cupiditate sapiente maiores iusto ducimus cum excepturi veritatis quia</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="n">
-        <v>78</v>
-      </c>
-      <c r="C79" t="n">
-        <v>18000</v>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>est minima eius possimus ea ratione velit et</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" t="n">
-        <v>79</v>
-      </c>
-      <c r="C80" t="n">
-        <v>19000</v>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>ipsa quae voluptas natus ut suscipit soluta quia quidem</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" t="n">
-        <v>80</v>
-      </c>
-      <c r="C81" t="n">
-        <v>20000</v>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>id nihil reprehenderit</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" t="n">
-        <v>81</v>
-      </c>
-      <c r="C82" t="n">
-        <v>21000</v>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>quibusdam sapiente et</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" t="n">
-        <v>82</v>
-      </c>
-      <c r="C83" t="n">
-        <v>22000</v>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>recusandae consequatur vel amet unde</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" t="n">
-        <v>83</v>
-      </c>
-      <c r="C84" t="n">
-        <v>23000</v>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>aperiam odio fugiat</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="B85" t="n">
-        <v>84</v>
-      </c>
-      <c r="C85" t="n">
-        <v>24000</v>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>est et at eos expedita</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="B86" t="n">
-        <v>85</v>
-      </c>
-      <c r="C86" t="n">
-        <v>25000</v>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>qui voluptatem consequatur aut ab quis temporibus praesentium</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="B87" t="n">
-        <v>86</v>
-      </c>
-      <c r="C87" t="n">
-        <v>26000</v>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>eligendi mollitia alias aspernatur vel ut iusto</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="B88" t="n">
-        <v>87</v>
-      </c>
-      <c r="C88" t="n">
-        <v>27000</v>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>aut aut architecto</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="B89" t="n">
-        <v>88</v>
-      </c>
-      <c r="C89" t="n">
-        <v>28000</v>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>quas perspiciatis optio</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="B90" t="n">
-        <v>89</v>
-      </c>
-      <c r="C90" t="n">
-        <v>29000</v>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>sit optio id voluptatem est eum et</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="B91" t="n">
-        <v>90</v>
-      </c>
-      <c r="C91" t="n">
-        <v>30000</v>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>est vel dignissimos</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="B92" t="n">
-        <v>91</v>
-      </c>
-      <c r="C92" t="n">
-        <v>31000</v>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>repellendus praesentium debitis officiis</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="B93" t="n">
-        <v>92</v>
-      </c>
-      <c r="C93" t="n">
-        <v>32000</v>
-      </c>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>incidunt et et eligendi assumenda soluta quia recusandae</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="B94" t="n">
-        <v>93</v>
-      </c>
-      <c r="C94" t="n">
-        <v>33000</v>
-      </c>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>nisi qui dolores perspiciatis</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="B95" t="n">
-        <v>94</v>
-      </c>
-      <c r="C95" t="n">
-        <v>34000</v>
-      </c>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>quisquam a dolores et earum vitae</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="B96" t="n">
-        <v>95</v>
-      </c>
-      <c r="C96" t="n">
-        <v>35000</v>
-      </c>
-      <c r="E96" t="inlineStr">
-        <is>
-          <t>consectetur vel rerum qui aperiam modi eos aspernatur ipsa</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="B97" t="n">
-        <v>96</v>
-      </c>
-      <c r="C97" t="n">
-        <v>36000</v>
-      </c>
-      <c r="E97" t="inlineStr">
-        <is>
-          <t>unde et ut molestiae est molestias voluptatem sint</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="B98" t="n">
-        <v>97</v>
-      </c>
-      <c r="C98" t="n">
-        <v>37000</v>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>est quod aut</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="B99" t="n">
-        <v>98</v>
-      </c>
-      <c r="C99" t="n">
-        <v>38000</v>
-      </c>
-      <c r="E99" t="inlineStr">
-        <is>
-          <t>omnis quia possimus nesciunt deleniti assumenda sed autem</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="B100" t="n">
-        <v>99</v>
-      </c>
-      <c r="C100" t="n">
-        <v>39000</v>
-      </c>
-      <c r="E100" t="inlineStr">
-        <is>
-          <t>consectetur ut id impedit dolores sit ad ex aut</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>